<commit_message>
IU, GET REPORT, EXCEL...
</commit_message>
<xml_diff>
--- a/src/main/resources/files/Conditions.xlsx
+++ b/src/main/resources/files/Conditions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ceu365-my.sharepoint.com/personal/maria_martinezlabrador_usp_ceu_es/Documents/DSS_Anemia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_7E4E55BF84DCCEE3ED7FF6F99031F45BFA722949" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F98F8B24-0058-4F4E-A01E-160EA330559E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A84061-0A22-40C1-A726-569BD8840BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,18 +44,12 @@
     <t>Hb</t>
   </si>
   <si>
-    <t xml:space="preserve">EPO </t>
-  </si>
-  <si>
     <t>Hematocrit/PVM</t>
   </si>
   <si>
     <t>Plaquets</t>
   </si>
   <si>
-    <t xml:space="preserve">Anisocytosis coefficient </t>
-  </si>
-  <si>
     <t>Reticulocytes</t>
   </si>
   <si>
@@ -71,9 +65,6 @@
     <t>RBC</t>
   </si>
   <si>
-    <t xml:space="preserve">VCM </t>
-  </si>
-  <si>
     <t>MCH</t>
   </si>
   <si>
@@ -92,30 +83,6 @@
     <t>Fe</t>
   </si>
   <si>
-    <t xml:space="preserve">Bilirubine </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDH </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Haptoglobin </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ferritin </t>
-  </si>
-  <si>
-    <t xml:space="preserve">B12 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Folic acid 			</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glucocorticoids </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skin paleness </t>
-  </si>
-  <si>
     <t>Tachycardia</t>
   </si>
   <si>
@@ -152,12 +119,6 @@
     <t>Cold hands/feet</t>
   </si>
   <si>
-    <t xml:space="preserve">Intern hemorrhage </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extern hemorrhage </t>
-  </si>
-  <si>
     <t>Nausea, poor apetite</t>
   </si>
   <si>
@@ -170,9 +131,6 @@
     <t>Craneal balloning</t>
   </si>
   <si>
-    <t xml:space="preserve">Aplastic crisis </t>
-  </si>
-  <si>
     <t>Bacterial infectons</t>
   </si>
   <si>
@@ -182,9 +140,6 @@
     <t>Bone deformations</t>
   </si>
   <si>
-    <t xml:space="preserve">Maxilar bone hyperplasia </t>
-  </si>
-  <si>
     <t>Brittle nails</t>
   </si>
   <si>
@@ -194,9 +149,6 @@
     <t>Diarrhea</t>
   </si>
   <si>
-    <t xml:space="preserve">Paresthesia </t>
-  </si>
-  <si>
     <t>Cyanosis</t>
   </si>
   <si>
@@ -206,12 +158,6 @@
     <t>Vomit</t>
   </si>
   <si>
-    <t xml:space="preserve">Petechiae </t>
-  </si>
-  <si>
-    <t>Anemic syndrome</t>
-  </si>
-  <si>
     <t>&lt;8</t>
   </si>
   <si>
@@ -221,9 +167,6 @@
     <t>TRUE</t>
   </si>
   <si>
-    <t>Posthemorrhagic anemia MALE</t>
-  </si>
-  <si>
     <t xml:space="preserve"> &gt;2.5</t>
   </si>
   <si>
@@ -239,15 +182,9 @@
     <t>&lt;60</t>
   </si>
   <si>
-    <t>Posthemorrhagic anemia FEMALE</t>
-  </si>
-  <si>
     <t>&lt;4.1</t>
   </si>
   <si>
-    <t>Hemolytic anemia MALE</t>
-  </si>
-  <si>
     <t>10-13.5</t>
   </si>
   <si>
@@ -272,27 +209,15 @@
     <t>&lt;41</t>
   </si>
   <si>
-    <t>Hemolytic anemia FEMALE</t>
-  </si>
-  <si>
     <t>10-12.3</t>
   </si>
   <si>
-    <t>Inherited spherocytosis</t>
-  </si>
-  <si>
     <t>&lt;80</t>
   </si>
   <si>
     <t>&gt;360</t>
   </si>
   <si>
-    <t>Thalassemia/Sicleform anemia</t>
-  </si>
-  <si>
-    <t>Iron-deficiency anemia MALE</t>
-  </si>
-  <si>
     <t>2.6-18.5</t>
   </si>
   <si>
@@ -311,12 +236,6 @@
     <t>&lt;12</t>
   </si>
   <si>
-    <t>Iron-deficiency anemia FEMALE</t>
-  </si>
-  <si>
-    <t>Megaloblastic anemia MALE</t>
-  </si>
-  <si>
     <t>&lt;7.4</t>
   </si>
   <si>
@@ -329,33 +248,15 @@
     <t>&lt;2.7</t>
   </si>
   <si>
-    <t>Megaloblastic anemia FEMALE</t>
-  </si>
-  <si>
-    <t>Aplasic anemia MALE</t>
-  </si>
-  <si>
-    <t>Aplasic anemia FEMALE</t>
-  </si>
-  <si>
     <t xml:space="preserve"> &lt;4.1</t>
   </si>
   <si>
-    <t>Chronic disease anemia MALE</t>
-  </si>
-  <si>
     <t xml:space="preserve"> &lt;2.6</t>
   </si>
   <si>
     <t>&gt;300</t>
   </si>
   <si>
-    <t>Chronic disease anemia FEMALE</t>
-  </si>
-  <si>
-    <t>Polycythemia MALE</t>
-  </si>
-  <si>
     <t>&gt;17.5</t>
   </si>
   <si>
@@ -368,9 +269,6 @@
     <t>&gt;25</t>
   </si>
   <si>
-    <t>Polycythemia FEMALE</t>
-  </si>
-  <si>
     <t>&gt;15.3</t>
   </si>
   <si>
@@ -378,6 +276,108 @@
   </si>
   <si>
     <t>&gt;5.3</t>
+  </si>
+  <si>
+    <t>Folic acid</t>
+  </si>
+  <si>
+    <t>Anemic_syndrome</t>
+  </si>
+  <si>
+    <t>Posthemorrhagic_anemia_MALE</t>
+  </si>
+  <si>
+    <t>Posthemorrhagic_anemia_FEMALE</t>
+  </si>
+  <si>
+    <t>Hemolytic_anemia_MALE</t>
+  </si>
+  <si>
+    <t>Hemolytic_anemia_FEMALE</t>
+  </si>
+  <si>
+    <t>Inherited_spherocytosis</t>
+  </si>
+  <si>
+    <t>Thalassemia/Sicleform_anemia</t>
+  </si>
+  <si>
+    <t>Megaloblastic_anemia_MALE</t>
+  </si>
+  <si>
+    <t>Megaloblastic_anemia_FEMALE</t>
+  </si>
+  <si>
+    <t>Aplasic_anemia_MALE</t>
+  </si>
+  <si>
+    <t>Aplasic_anemia_FEMALE</t>
+  </si>
+  <si>
+    <t>Chronic_disease_anemia_MALE</t>
+  </si>
+  <si>
+    <t>Chronic_disease_anemia_FEMALE</t>
+  </si>
+  <si>
+    <t>Polycythemia_MALE</t>
+  </si>
+  <si>
+    <t>Polycythemia_FEMALE</t>
+  </si>
+  <si>
+    <t>Iron_deficiency_anemia_MALE</t>
+  </si>
+  <si>
+    <t>Iron_deficiency_anemia_FEMALE</t>
+  </si>
+  <si>
+    <t>EPO</t>
+  </si>
+  <si>
+    <t>Anisocytosis coefficient</t>
+  </si>
+  <si>
+    <t>VCM</t>
+  </si>
+  <si>
+    <t>Bilirubine</t>
+  </si>
+  <si>
+    <t>LDH</t>
+  </si>
+  <si>
+    <t>Haptoglobin</t>
+  </si>
+  <si>
+    <t>Ferritin</t>
+  </si>
+  <si>
+    <t>B12</t>
+  </si>
+  <si>
+    <t>Glucocorticoids</t>
+  </si>
+  <si>
+    <t>Skin paleness</t>
+  </si>
+  <si>
+    <t>Intern hemorrhage</t>
+  </si>
+  <si>
+    <t>Extern hemorrhage</t>
+  </si>
+  <si>
+    <t>Aplastic crisis</t>
+  </si>
+  <si>
+    <t>Maxilar bone hyperplasia</t>
+  </si>
+  <si>
+    <t>Paresthesia</t>
+  </si>
+  <si>
+    <t>Petechiae</t>
   </si>
 </sst>
 </file>
@@ -1291,13 +1291,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BE18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="BB1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="BE1" sqref="BE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="57" width="35.77734375" customWidth="1"/>
+    <col min="1" max="1" width="41.109375" customWidth="1"/>
+    <col min="2" max="57" width="35.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:57" ht="19.95" customHeight="1">
@@ -1308,180 +1309,180 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="R1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="S1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="AB1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="AD1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="AE1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="AF1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="AG1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="AH1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AI1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AK1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AL1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AO1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AR1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AS1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AT1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AU1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AV1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AW1" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AX1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AY1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="BA1" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="BB1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="BC1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="BD1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AR1" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="AS1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="AT1" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="AU1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="AV1" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="AW1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="AX1" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="AY1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="AZ1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BA1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="BB1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="BC1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="BD1" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="BE1" s="3" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:57" ht="19.95" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
@@ -1506,43 +1507,43 @@
       <c r="X2" s="13"/>
       <c r="Y2" s="14"/>
       <c r="Z2" s="15" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AA2" s="16" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AB2" s="17" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AC2" s="17" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AD2" s="15" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AE2" s="17" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AF2" s="15" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AG2" s="17" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AH2" s="15" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AI2" s="17" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AJ2" s="15" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AK2" s="17" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AL2" s="15" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AM2" s="17"/>
       <c r="AN2" s="15"/>
@@ -1566,7 +1567,7 @@
     </row>
     <row r="3" spans="1:57" ht="19.95" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="19"/>
@@ -1574,28 +1575,28 @@
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="H3" s="19"/>
       <c r="I3" s="20"/>
       <c r="J3" s="19" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="L3" s="18" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="M3" s="18"/>
       <c r="N3" s="21" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="O3" s="18"/>
       <c r="P3" s="19"/>
       <c r="Q3" s="18"/>
       <c r="R3" s="19" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="S3" s="19"/>
       <c r="T3" s="22"/>
@@ -1605,35 +1606,35 @@
       <c r="X3" s="22"/>
       <c r="Y3" s="23"/>
       <c r="Z3" s="24" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AA3" s="24" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AB3" s="25"/>
       <c r="AC3" s="25"/>
       <c r="AD3" s="24"/>
       <c r="AE3" s="25" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AF3" s="24"/>
       <c r="AG3" s="25"/>
       <c r="AH3" s="26" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AI3" s="25"/>
       <c r="AJ3" s="24" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AK3" s="25" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AL3" s="24"/>
       <c r="AM3" s="25" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AN3" s="24" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AO3" s="25"/>
       <c r="AP3" s="25"/>
@@ -1655,7 +1656,7 @@
     </row>
     <row r="4" spans="1:57" ht="19.95" customHeight="1">
       <c r="A4" s="8" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="19"/>
@@ -1663,28 +1664,28 @@
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
       <c r="G4" s="19" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="H4" s="19"/>
       <c r="I4" s="20"/>
       <c r="J4" s="19" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="L4" s="18" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="M4" s="18"/>
       <c r="N4" s="21" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="O4" s="18"/>
       <c r="P4" s="19"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="19" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="S4" s="19"/>
       <c r="T4" s="22"/>
@@ -1694,35 +1695,35 @@
       <c r="X4" s="22"/>
       <c r="Y4" s="23"/>
       <c r="Z4" s="27" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AA4" s="27" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AB4" s="28"/>
       <c r="AC4" s="28"/>
       <c r="AD4" s="27"/>
       <c r="AE4" s="28" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AF4" s="27"/>
       <c r="AG4" s="28"/>
       <c r="AH4" s="29" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AI4" s="28"/>
       <c r="AJ4" s="27" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AK4" s="28" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AL4" s="27"/>
       <c r="AM4" s="28" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AN4" s="27" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AO4" s="28"/>
       <c r="AP4" s="28"/>
@@ -1744,62 +1745,62 @@
     </row>
     <row r="5" spans="1:57" ht="19.95" customHeight="1">
       <c r="A5" s="8" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D5" s="31"/>
       <c r="E5" s="31"/>
       <c r="F5" s="31"/>
       <c r="G5" s="31" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="H5" s="32" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="I5" s="33"/>
       <c r="J5" s="31"/>
       <c r="K5" s="30" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="L5" s="30" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="M5" s="30" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="N5" s="30" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="O5" s="30"/>
       <c r="P5" s="30" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="Q5" s="30" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="R5" s="34" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="S5" s="34" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="T5" s="30" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="U5" s="34" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="V5" s="35"/>
       <c r="W5" s="36"/>
       <c r="X5" s="35"/>
       <c r="Y5" s="36"/>
       <c r="Z5" s="37" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AA5" s="37"/>
       <c r="AB5" s="38"/>
@@ -1809,7 +1810,7 @@
       <c r="AF5" s="37"/>
       <c r="AG5" s="38"/>
       <c r="AH5" s="37" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AI5" s="38"/>
       <c r="AJ5" s="37"/>
@@ -1819,16 +1820,16 @@
       <c r="AN5" s="37"/>
       <c r="AO5" s="38"/>
       <c r="AP5" s="39" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AQ5" s="40" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AR5" s="37" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AS5" s="37" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AT5" s="38"/>
       <c r="AU5" s="37"/>
@@ -1845,62 +1846,62 @@
     </row>
     <row r="6" spans="1:57" ht="19.95" customHeight="1">
       <c r="A6" s="8" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="31"/>
       <c r="F6" s="31"/>
       <c r="G6" s="31" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="I6" s="30"/>
       <c r="J6" s="31"/>
       <c r="K6" s="31" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="L6" s="30" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="M6" s="30" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="N6" s="42" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="31" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="Q6" s="30" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="R6" s="34" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="S6" s="34" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="T6" s="30" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="U6" s="34" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="V6" s="35"/>
       <c r="W6" s="36"/>
       <c r="X6" s="35"/>
       <c r="Y6" s="36"/>
       <c r="Z6" s="37" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AA6" s="37"/>
       <c r="AB6" s="38"/>
@@ -1910,7 +1911,7 @@
       <c r="AF6" s="37"/>
       <c r="AG6" s="38"/>
       <c r="AH6" s="37" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AI6" s="38"/>
       <c r="AJ6" s="37"/>
@@ -1920,16 +1921,16 @@
       <c r="AN6" s="37"/>
       <c r="AO6" s="38"/>
       <c r="AP6" s="43" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AQ6" s="40" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AR6" s="38" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AS6" s="37" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AT6" s="38"/>
       <c r="AU6" s="37"/>
@@ -1946,7 +1947,7 @@
     </row>
     <row r="7" spans="1:57" ht="19.95" customHeight="1">
       <c r="A7" s="8" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B7" s="44"/>
       <c r="C7" s="45"/>
@@ -1954,28 +1955,28 @@
       <c r="E7" s="45"/>
       <c r="F7" s="45"/>
       <c r="G7" s="45" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="H7" s="45"/>
       <c r="I7" s="44"/>
       <c r="J7" s="45"/>
       <c r="K7" s="45"/>
       <c r="L7" s="44" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="M7" s="44"/>
       <c r="N7" s="46" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="O7" s="44"/>
       <c r="P7" s="45"/>
       <c r="Q7" s="44"/>
       <c r="R7" s="45"/>
       <c r="S7" s="47" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="T7" s="44" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="U7" s="45"/>
       <c r="V7" s="48"/>
@@ -1999,28 +2000,28 @@
       <c r="AN7" s="50"/>
       <c r="AO7" s="51"/>
       <c r="AP7" s="52" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AQ7" s="51" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AR7" s="53" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AS7" s="50" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AT7" s="51" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AU7" s="50" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AV7" s="51" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AW7" s="54" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AX7" s="51"/>
       <c r="AY7" s="50"/>
@@ -2033,7 +2034,7 @@
     </row>
     <row r="8" spans="1:57" ht="19.95" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B8" s="55"/>
       <c r="C8" s="56"/>
@@ -2046,11 +2047,11 @@
       <c r="J8" s="56"/>
       <c r="K8" s="56"/>
       <c r="L8" s="55" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="M8" s="55"/>
       <c r="N8" s="57" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="O8" s="55"/>
       <c r="P8" s="56"/>
@@ -2064,10 +2065,10 @@
       <c r="X8" s="58"/>
       <c r="Y8" s="59"/>
       <c r="Z8" s="60" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AA8" s="55" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AB8" s="56"/>
       <c r="AC8" s="56"/>
@@ -2075,23 +2076,23 @@
       <c r="AE8" s="56"/>
       <c r="AF8" s="55"/>
       <c r="AG8" s="56" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AH8" s="55" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AI8" s="56"/>
       <c r="AJ8" s="55" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AK8" s="56"/>
       <c r="AL8" s="55" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AM8" s="56"/>
       <c r="AN8" s="55"/>
       <c r="AO8" s="56" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AP8" s="56"/>
       <c r="AQ8" s="55"/>
@@ -2100,14 +2101,14 @@
       <c r="AT8" s="56"/>
       <c r="AU8" s="55"/>
       <c r="AV8" s="61" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AW8" s="55"/>
       <c r="AX8" s="56" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AY8" s="57" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AZ8" s="56"/>
       <c r="BA8" s="55"/>
@@ -2118,50 +2119,50 @@
     </row>
     <row r="9" spans="1:57" ht="19.95" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="B9" s="62" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="C9" s="63" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="G9" s="47" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="12"/>
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
       <c r="L9" s="12" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="M9" s="21" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="N9" s="12"/>
       <c r="O9" s="12"/>
       <c r="P9" s="11"/>
       <c r="Q9" s="12"/>
       <c r="R9" s="11" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="S9" s="11"/>
       <c r="T9" s="13"/>
       <c r="U9" s="14"/>
       <c r="V9" s="21" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="W9" s="14"/>
       <c r="X9" s="13"/>
       <c r="Y9" s="14"/>
       <c r="Z9" s="29" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AA9" s="12"/>
       <c r="AB9" s="11"/>
@@ -2171,11 +2172,11 @@
       <c r="AF9" s="12"/>
       <c r="AG9" s="11"/>
       <c r="AH9" s="12" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AI9" s="11"/>
       <c r="AJ9" s="12" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AK9" s="11"/>
       <c r="AL9" s="12"/>
@@ -2193,10 +2194,10 @@
       <c r="AX9" s="11"/>
       <c r="AY9" s="12"/>
       <c r="AZ9" s="11" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="BA9" s="12" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="BB9" s="12"/>
       <c r="BC9" s="12"/>
@@ -2205,50 +2206,50 @@
     </row>
     <row r="10" spans="1:57" ht="19.95" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B10" s="64" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="G10" s="47" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="12"/>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
       <c r="L10" s="12" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="M10" s="21" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
       <c r="P10" s="11"/>
       <c r="Q10" s="12"/>
       <c r="R10" s="11" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="S10" s="11"/>
       <c r="T10" s="13"/>
       <c r="U10" s="14"/>
       <c r="V10" s="21" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="W10" s="14"/>
       <c r="X10" s="13"/>
       <c r="Y10" s="14"/>
       <c r="Z10" s="29" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AA10" s="12"/>
       <c r="AB10" s="11"/>
@@ -2258,11 +2259,11 @@
       <c r="AF10" s="12"/>
       <c r="AG10" s="11"/>
       <c r="AH10" s="12" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AI10" s="11"/>
       <c r="AJ10" s="12" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AK10" s="11"/>
       <c r="AL10" s="12"/>
@@ -2280,10 +2281,10 @@
       <c r="AX10" s="11"/>
       <c r="AY10" s="12"/>
       <c r="AZ10" s="11" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="BA10" s="12" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="BB10" s="12"/>
       <c r="BC10" s="12"/>
@@ -2292,32 +2293,32 @@
     </row>
     <row r="11" spans="1:57" ht="19.95" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
       <c r="E11" s="19" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="G11" s="19"/>
       <c r="H11" s="19" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="I11" s="18"/>
       <c r="J11" s="19"/>
       <c r="K11" s="19" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="L11" s="18" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="M11" s="18"/>
       <c r="N11" s="18" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="O11" s="18"/>
       <c r="P11" s="19"/>
@@ -2328,14 +2329,14 @@
       <c r="U11" s="23"/>
       <c r="V11" s="22"/>
       <c r="W11" s="47" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="X11" s="21" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="Y11" s="23"/>
       <c r="Z11" s="65" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AA11" s="18"/>
       <c r="AB11" s="19"/>
@@ -2345,7 +2346,7 @@
       <c r="AF11" s="18"/>
       <c r="AG11" s="19"/>
       <c r="AH11" s="66" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AI11" s="19"/>
       <c r="AJ11" s="18"/>
@@ -2364,7 +2365,7 @@
       <c r="AW11" s="18"/>
       <c r="AX11" s="19"/>
       <c r="AY11" s="18" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AZ11" s="19"/>
       <c r="BA11" s="18"/>
@@ -2372,37 +2373,37 @@
       <c r="BC11" s="18"/>
       <c r="BD11" s="18"/>
       <c r="BE11" s="19" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:57" ht="19.95" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
       <c r="E12" s="19" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="19" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="I12" s="18"/>
       <c r="J12" s="19"/>
       <c r="K12" s="19" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="L12" s="18" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="M12" s="18"/>
       <c r="N12" s="18" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="O12" s="18"/>
       <c r="P12" s="19"/>
@@ -2413,14 +2414,14 @@
       <c r="U12" s="23"/>
       <c r="V12" s="22"/>
       <c r="W12" s="47" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="X12" s="21" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="Y12" s="23"/>
       <c r="Z12" s="65" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AA12" s="18"/>
       <c r="AB12" s="19"/>
@@ -2430,7 +2431,7 @@
       <c r="AF12" s="18"/>
       <c r="AG12" s="19"/>
       <c r="AH12" s="66" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AI12" s="19"/>
       <c r="AJ12" s="18"/>
@@ -2449,7 +2450,7 @@
       <c r="AW12" s="18"/>
       <c r="AX12" s="19"/>
       <c r="AY12" s="18" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AZ12" s="19"/>
       <c r="BA12" s="18"/>
@@ -2457,28 +2458,28 @@
       <c r="BC12" s="18"/>
       <c r="BD12" s="18"/>
       <c r="BE12" s="18" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:57" ht="19.95" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B13" s="67"/>
       <c r="C13" s="68"/>
       <c r="D13" s="68"/>
       <c r="E13" s="47" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="F13" s="68"/>
       <c r="G13" s="68"/>
       <c r="H13" s="47" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="I13" s="67"/>
       <c r="J13" s="68"/>
       <c r="K13" s="21" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="L13" s="67"/>
       <c r="M13" s="67"/>
@@ -2495,7 +2496,7 @@
       <c r="X13" s="69"/>
       <c r="Y13" s="70"/>
       <c r="Z13" s="71" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AA13" s="67"/>
       <c r="AB13" s="68"/>
@@ -2504,22 +2505,22 @@
       <c r="AE13" s="68"/>
       <c r="AF13" s="67"/>
       <c r="AG13" s="68" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AH13" s="67" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AI13" s="68"/>
       <c r="AJ13" s="67" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AK13" s="68"/>
       <c r="AL13" s="67"/>
       <c r="AM13" s="61" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AN13" s="66" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AO13" s="68"/>
       <c r="AP13" s="68"/>
@@ -2541,23 +2542,23 @@
     </row>
     <row r="14" spans="1:57" ht="19.95" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B14" s="67"/>
       <c r="C14" s="68"/>
       <c r="D14" s="68"/>
       <c r="E14" s="47" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="F14" s="68"/>
       <c r="G14" s="68"/>
       <c r="H14" s="47" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="I14" s="67"/>
       <c r="J14" s="68"/>
       <c r="K14" s="47" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="L14" s="67"/>
       <c r="M14" s="67"/>
@@ -2574,7 +2575,7 @@
       <c r="X14" s="69"/>
       <c r="Y14" s="70"/>
       <c r="Z14" s="71" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AA14" s="67"/>
       <c r="AB14" s="68"/>
@@ -2583,22 +2584,22 @@
       <c r="AE14" s="68"/>
       <c r="AF14" s="67"/>
       <c r="AG14" s="68" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AH14" s="67" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AI14" s="68"/>
       <c r="AJ14" s="67" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AK14" s="68"/>
       <c r="AL14" s="67"/>
       <c r="AM14" s="61" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AN14" s="66" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AO14" s="68"/>
       <c r="AP14" s="68"/>
@@ -2620,24 +2621,24 @@
     </row>
     <row r="15" spans="1:57" ht="19.95" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B15" s="44"/>
       <c r="C15" s="21" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="D15" s="45"/>
       <c r="E15" s="45"/>
       <c r="F15" s="45"/>
       <c r="G15" s="45" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="H15" s="45"/>
       <c r="I15" s="44"/>
       <c r="J15" s="45"/>
       <c r="K15" s="45"/>
       <c r="L15" s="44" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="M15" s="44"/>
       <c r="N15" s="44"/>
@@ -2645,19 +2646,19 @@
       <c r="P15" s="45"/>
       <c r="Q15" s="44"/>
       <c r="R15" s="45" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="S15" s="45"/>
       <c r="T15" s="48"/>
       <c r="U15" s="49"/>
       <c r="V15" s="72" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="W15" s="49"/>
       <c r="X15" s="48"/>
       <c r="Y15" s="49"/>
       <c r="Z15" s="29" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AA15" s="44"/>
       <c r="AB15" s="45"/>
@@ -2666,12 +2667,12 @@
       <c r="AE15" s="45"/>
       <c r="AF15" s="44"/>
       <c r="AG15" s="45" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AH15" s="44"/>
       <c r="AI15" s="45"/>
       <c r="AJ15" s="44" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AK15" s="45"/>
       <c r="AL15" s="44"/>
@@ -2697,24 +2698,24 @@
     </row>
     <row r="16" spans="1:57" ht="19.95" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B16" s="44"/>
       <c r="C16" s="47" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="D16" s="45"/>
       <c r="E16" s="45"/>
       <c r="F16" s="45"/>
       <c r="G16" s="45" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="H16" s="45"/>
       <c r="I16" s="44"/>
       <c r="J16" s="45"/>
       <c r="K16" s="45"/>
       <c r="L16" s="44" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="M16" s="44"/>
       <c r="N16" s="44"/>
@@ -2722,19 +2723,19 @@
       <c r="P16" s="45"/>
       <c r="Q16" s="44"/>
       <c r="R16" s="45" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="S16" s="45"/>
       <c r="T16" s="48"/>
       <c r="U16" s="49"/>
       <c r="V16" s="72" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="W16" s="49"/>
       <c r="X16" s="48"/>
       <c r="Y16" s="49"/>
       <c r="Z16" s="29" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AA16" s="44"/>
       <c r="AB16" s="45"/>
@@ -2743,12 +2744,12 @@
       <c r="AE16" s="45"/>
       <c r="AF16" s="44"/>
       <c r="AG16" s="45" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AH16" s="44"/>
       <c r="AI16" s="45"/>
       <c r="AJ16" s="44" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AK16" s="45"/>
       <c r="AL16" s="44"/>
@@ -2774,27 +2775,27 @@
     </row>
     <row r="17" spans="1:57" ht="19.95" customHeight="1">
       <c r="A17" s="8" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="C17" s="73" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="E17" s="74"/>
       <c r="F17" s="74"/>
       <c r="G17" s="74"/>
       <c r="H17" s="74"/>
       <c r="I17" s="66" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="J17" s="74"/>
       <c r="K17" s="47" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="L17" s="75"/>
       <c r="M17" s="75"/>
@@ -2810,7 +2811,7 @@
       <c r="W17" s="77"/>
       <c r="X17" s="76"/>
       <c r="Y17" s="47" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="Z17" s="78"/>
       <c r="AA17" s="75"/>
@@ -2819,10 +2820,10 @@
       <c r="AD17" s="75"/>
       <c r="AE17" s="74"/>
       <c r="AF17" s="75" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AG17" s="74" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AH17" s="75"/>
       <c r="AI17" s="74"/>
@@ -2831,7 +2832,7 @@
       <c r="AL17" s="75"/>
       <c r="AM17" s="74"/>
       <c r="AN17" s="75" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AO17" s="74"/>
       <c r="AP17" s="74"/>
@@ -2845,43 +2846,43 @@
       <c r="AX17" s="74"/>
       <c r="AY17" s="75"/>
       <c r="AZ17" s="74" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="BA17" s="75"/>
       <c r="BB17" s="75" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="BC17" s="75" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="BD17" s="75" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="BE17" s="74"/>
     </row>
     <row r="18" spans="1:57" ht="19.95" customHeight="1">
       <c r="A18" s="79" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="C18" s="80" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D18" s="81" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="E18" s="82"/>
       <c r="F18" s="82"/>
       <c r="G18" s="82"/>
       <c r="H18" s="82"/>
       <c r="I18" s="83" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="J18" s="82"/>
       <c r="K18" s="81" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="L18" s="84"/>
       <c r="M18" s="84"/>
@@ -2897,7 +2898,7 @@
       <c r="W18" s="82"/>
       <c r="X18" s="84"/>
       <c r="Y18" s="81" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="Z18" s="85"/>
       <c r="AA18" s="85"/>
@@ -2906,10 +2907,10 @@
       <c r="AD18" s="85"/>
       <c r="AE18" s="86"/>
       <c r="AF18" s="84" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AG18" s="82" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AH18" s="85"/>
       <c r="AI18" s="86"/>
@@ -2918,7 +2919,7 @@
       <c r="AL18" s="85"/>
       <c r="AM18" s="86"/>
       <c r="AN18" s="87" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="AO18" s="86"/>
       <c r="AP18" s="86"/>
@@ -2932,17 +2933,17 @@
       <c r="AX18" s="86"/>
       <c r="AY18" s="85"/>
       <c r="AZ18" s="88" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="BA18" s="85"/>
       <c r="BB18" s="84" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="BC18" s="84" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="BD18" s="84" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="BE18" s="86"/>
     </row>

</xml_diff>

<commit_message>
jar menu user man xlxs
</commit_message>
<xml_diff>
--- a/src/main/resources/files/Conditions.xlsx
+++ b/src/main/resources/files/Conditions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\IdeaProjects\AnemiaDSS\src\main\resources\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natalia/Documents/CEU/Asignaturas/SistemasSoporte/AnemiaDSS/src/main/resources/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A559176A-153C-4B97-8C4C-F446A212C08C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5237C325-5BE8-C042-B63A-5FCFA2566089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -390,7 +390,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1433,17 +1433,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="AY1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="BD1" sqref="BD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.109375" customWidth="1"/>
-    <col min="2" max="56" width="35.77734375" customWidth="1"/>
+    <col min="1" max="1" width="41.1640625" customWidth="1"/>
+    <col min="2" max="56" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="19.95" customHeight="1">
+    <row r="1" spans="1:56" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:56" ht="19.95" customHeight="1">
+    <row r="2" spans="1:56" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>101</v>
       </c>
@@ -1703,7 +1703,7 @@
       <c r="BC2" s="92"/>
       <c r="BD2" s="91"/>
     </row>
-    <row r="3" spans="1:56" ht="19.95" customHeight="1">
+    <row r="3" spans="1:56" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>102</v>
       </c>
@@ -1793,7 +1793,7 @@
       <c r="BC3" s="92"/>
       <c r="BD3" s="91"/>
     </row>
-    <row r="4" spans="1:56" ht="19.95" customHeight="1">
+    <row r="4" spans="1:56" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>75</v>
       </c>
@@ -1881,7 +1881,7 @@
       <c r="BC4" s="23"/>
       <c r="BD4" s="24"/>
     </row>
-    <row r="5" spans="1:56" ht="19.95" customHeight="1">
+    <row r="5" spans="1:56" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>76</v>
       </c>
@@ -1969,7 +1969,7 @@
       <c r="BC5" s="26"/>
       <c r="BD5" s="27"/>
     </row>
-    <row r="6" spans="1:56" ht="19.95" customHeight="1">
+    <row r="6" spans="1:56" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>77</v>
       </c>
@@ -2069,7 +2069,7 @@
       <c r="BC6" s="36"/>
       <c r="BD6" s="37"/>
     </row>
-    <row r="7" spans="1:56" ht="19.95" customHeight="1">
+    <row r="7" spans="1:56" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>78</v>
       </c>
@@ -2169,7 +2169,7 @@
       <c r="BC7" s="36"/>
       <c r="BD7" s="37"/>
     </row>
-    <row r="8" spans="1:56" ht="19.95" customHeight="1">
+    <row r="8" spans="1:56" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>104</v>
       </c>
@@ -2255,7 +2255,7 @@
       <c r="BC8" s="49"/>
       <c r="BD8" s="50"/>
     </row>
-    <row r="9" spans="1:56" ht="19.95" customHeight="1">
+    <row r="9" spans="1:56" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>103</v>
       </c>
@@ -2337,7 +2337,7 @@
       <c r="BC9" s="49"/>
       <c r="BD9" s="50"/>
     </row>
-    <row r="10" spans="1:56" ht="19.95" customHeight="1">
+    <row r="10" spans="1:56" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>105</v>
       </c>
@@ -2421,7 +2421,7 @@
       <c r="BC10" s="54"/>
       <c r="BD10" s="55"/>
     </row>
-    <row r="11" spans="1:56" ht="19.95" customHeight="1">
+    <row r="11" spans="1:56" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>106</v>
       </c>
@@ -2505,7 +2505,7 @@
       <c r="BC11" s="54"/>
       <c r="BD11" s="55"/>
     </row>
-    <row r="12" spans="1:56" ht="19.95" customHeight="1">
+    <row r="12" spans="1:56" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>85</v>
       </c>
@@ -2591,7 +2591,7 @@
       <c r="BC12" s="11"/>
       <c r="BD12" s="10"/>
     </row>
-    <row r="13" spans="1:56" ht="19.95" customHeight="1">
+    <row r="13" spans="1:56" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>86</v>
       </c>
@@ -2677,7 +2677,7 @@
       <c r="BC13" s="11"/>
       <c r="BD13" s="10"/>
     </row>
-    <row r="14" spans="1:56" ht="19.95" customHeight="1">
+    <row r="14" spans="1:56" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>79</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:56" ht="19.95" customHeight="1">
+    <row r="15" spans="1:56" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>80</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:56" ht="19.95" customHeight="1">
+    <row r="16" spans="1:56" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>114</v>
       </c>
@@ -2923,7 +2923,7 @@
       <c r="BC16" s="104"/>
       <c r="BD16" s="103"/>
     </row>
-    <row r="17" spans="1:56" ht="19.95" customHeight="1">
+    <row r="17" spans="1:56" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>115</v>
       </c>
@@ -3001,7 +3001,7 @@
       <c r="BC17" s="104"/>
       <c r="BD17" s="103"/>
     </row>
-    <row r="18" spans="1:56" ht="19.95" customHeight="1">
+    <row r="18" spans="1:56" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>81</v>
       </c>
@@ -3077,7 +3077,7 @@
       <c r="BC18" s="43"/>
       <c r="BD18" s="44"/>
     </row>
-    <row r="19" spans="1:56" ht="19.95" customHeight="1">
+    <row r="19" spans="1:56" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>82</v>
       </c>
@@ -3153,7 +3153,7 @@
       <c r="BC19" s="43"/>
       <c r="BD19" s="44"/>
     </row>
-    <row r="20" spans="1:56" ht="19.95" customHeight="1">
+    <row r="20" spans="1:56" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>83</v>
       </c>
@@ -3239,7 +3239,7 @@
       </c>
       <c r="BD20" s="68"/>
     </row>
-    <row r="21" spans="1:56" ht="19.95" customHeight="1">
+    <row r="21" spans="1:56" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="73" t="s">
         <v>84</v>
       </c>
@@ -3325,7 +3325,7 @@
       </c>
       <c r="BD21" s="80"/>
     </row>
-    <row r="25" spans="1:56">
+    <row r="25" spans="1:56" x14ac:dyDescent="0.2">
       <c r="N25" s="84"/>
     </row>
   </sheetData>

</xml_diff>